<commit_message>
Under development file kiosk-1 version 1.1
</commit_message>
<xml_diff>
--- a/Electronics-Estimation.xlsx
+++ b/Electronics-Estimation.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kiosk-2_12-boxes" sheetId="3" r:id="rId2"/>
+    <sheet name="Kiosk-3_12-boxes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>Sno</t>
   </si>
@@ -155,6 +157,96 @@
   </si>
   <si>
     <t>Cost(INR)</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>PCB - Main</t>
+  </si>
+  <si>
+    <t>Arduino Mega Original</t>
+  </si>
+  <si>
+    <t>PCB OPTO</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>PCB DRIVER IC</t>
+  </si>
+  <si>
+    <t>PCB Mux</t>
+  </si>
+  <si>
+    <t>Connector Pair</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Arduino Cable</t>
+  </si>
+  <si>
+    <t>Light PCB</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Temperature Module</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor</t>
+  </si>
+  <si>
+    <t>Aviation Connector</t>
+  </si>
+  <si>
+    <t>Cables</t>
+  </si>
+  <si>
+    <t>2-pin plug Connector</t>
+  </si>
+  <si>
+    <t>3-pin plug Connector</t>
+  </si>
+  <si>
+    <t>4-pin plug Connector</t>
+  </si>
+  <si>
+    <t>MCB</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>10.1inch Display</t>
+  </si>
+  <si>
+    <t>DP to HDMI Connector</t>
+  </si>
+  <si>
+    <t>WIFI Adapter</t>
+  </si>
+  <si>
+    <t>Relay Board</t>
+  </si>
+  <si>
+    <t>SMPS</t>
   </si>
 </sst>
 </file>
@@ -257,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -303,6 +395,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -991,4 +1086,1094 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="13.54296875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1425</v>
+      </c>
+      <c r="E2" s="8">
+        <f>C2*D2</f>
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2700</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E27" si="0">C3*D3</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="8">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8">
+        <v>75</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>60</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8">
+        <v>15</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>50</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>200</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>200</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>200</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="8">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8">
+        <f>(150*0.18)+150</f>
+        <v>177</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8">
+        <v>12</v>
+      </c>
+      <c r="D14" s="8">
+        <v>750</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8">
+        <v>16</v>
+      </c>
+      <c r="D15" s="8">
+        <v>80</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="8">
+        <v>180</v>
+      </c>
+      <c r="D16" s="8">
+        <v>8</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="8">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8">
+        <v>110</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="8">
+        <v>15</v>
+      </c>
+      <c r="D18" s="8">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="8">
+        <v>8</v>
+      </c>
+      <c r="D19" s="8">
+        <v>8</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="8">
+        <v>8</v>
+      </c>
+      <c r="D20" s="8">
+        <v>10</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2</v>
+      </c>
+      <c r="D21" s="8">
+        <v>140</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2</v>
+      </c>
+      <c r="D24" s="8">
+        <v>250</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8">
+        <v>600</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2800</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1200</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="8">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="8">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="3">
+        <f>SUM(E2:E31)</f>
+        <v>48523</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="13.54296875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1425</v>
+      </c>
+      <c r="E2" s="8">
+        <f>C2*D2</f>
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2700</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E27" si="0">C3*D3</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="8">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8">
+        <v>75</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>60</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8">
+        <v>15</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>50</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>200</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>200</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>200</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="8">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8">
+        <f>(135*0.18)+135</f>
+        <v>159.30000000000001</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>1911.6000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8">
+        <v>12</v>
+      </c>
+      <c r="D14" s="8">
+        <v>750</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8">
+        <v>16</v>
+      </c>
+      <c r="D15" s="8">
+        <v>80</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="8">
+        <v>18</v>
+      </c>
+      <c r="D16" s="8">
+        <v>110</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" ref="E16:E25" si="1">C16*D16</f>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="8">
+        <v>15</v>
+      </c>
+      <c r="D17" s="8">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="8">
+        <v>8</v>
+      </c>
+      <c r="D18" s="8">
+        <v>8</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="8">
+        <v>8</v>
+      </c>
+      <c r="D19" s="8">
+        <v>10</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2</v>
+      </c>
+      <c r="D20" s="8">
+        <v>140</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>12000</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>250</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8">
+        <v>4000</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1200</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="8">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="8">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="3">
+        <f>SUM(E2:E31)</f>
+        <v>49470.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>